<commit_message>
add item in table
</commit_message>
<xml_diff>
--- a/Парфюмерия.xlsx
+++ b/Парфюмерия.xlsx
@@ -4801,7 +4801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR6"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -5236,43 +5236,432 @@
       <c r="AR3" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="inlineStr"/>
-      <c r="AM6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="AM7" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Dilis Unique Sunny Туалетная вода 100 мл</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 088  </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 690 </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>13%</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>215973958</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Туалетная вода</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>